<commit_message>
remove files for clarity
</commit_message>
<xml_diff>
--- a/tornado plot.xlsx
+++ b/tornado plot.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a1b6ba592580725c/Desktop/GitHub/thermal-matlab/Optimization Example/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a1b6ba592580725c/Desktop/GitHub/thermal-matlab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="147" documentId="8_{8D10CBAF-EF6B-4BCA-97DD-A36551D6101E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4863BA86-24F9-41AE-A915-C59034526CF9}"/>
+  <xr:revisionPtr revIDLastSave="149" documentId="8_{8D10CBAF-EF6B-4BCA-97DD-A36551D6101E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E99E2D17-2CA5-4380-84C6-B591C2A7990A}"/>
   <bookViews>
-    <workbookView xWindow="1590" yWindow="1950" windowWidth="25980" windowHeight="13395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1607,8 +1607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>